<commit_message>
Minor code clean up and reorganization.
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE03175-B781-4248-A3B5-E3BD11148437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFCAA08-215B-480E-89F6-1F7935D73C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-270" yWindow="360" windowWidth="28470" windowHeight="15240" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1417,6 +1417,9 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>some submeshes aren't drawing, it seems</t>
   </si>
 </sst>
 </file>
@@ -2031,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,7 +2046,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2082,7 +2085,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2124,7 +2127,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -2162,8 +2165,11 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -2184,8 +2190,11 @@
       <c r="C11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>41</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Moved the parsing and Game Level data over to the renderer for efficiency. Partial implementation of level swap.
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFCAA08-215B-480E-89F6-1F7935D73C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323CD66D-E0A1-42C5-92B6-DB3AFBC4DAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-270" yWindow="360" windowWidth="28470" windowHeight="15240" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="30" yWindow="195" windowWidth="28470" windowHeight="15240" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1419,7 +1419,10 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>some submeshes aren't drawing, it seems</t>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Partially complete, some submeshes aren't drawing, it seems</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2040,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,8 +2168,8 @@
       <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>50</v>
+      <c r="D9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2228,6 +2231,9 @@
       <c r="C14" s="3">
         <v>0</v>
       </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -2239,6 +2245,9 @@
       <c r="C15" s="3">
         <v>0</v>
       </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -2251,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>7</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
@@ -2273,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -2305,8 +2314,11 @@
       <c r="C21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>12</v>
       </c>
@@ -2317,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>34</v>
       </c>
@@ -2328,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>47</v>
       </c>
@@ -2339,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
@@ -2350,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
@@ -2362,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2373,7 +2385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>48</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
@@ -2395,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>21</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
@@ -2417,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Levels can now be hotswapped
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323CD66D-E0A1-42C5-92B6-DB3AFBC4DAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB20614-DFB4-4351-9AC3-3AFEBAD31CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="195" windowWidth="28470" windowHeight="15240" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2039,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced broken assets from scene 1
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB20614-DFB4-4351-9AC3-3AFEBAD31CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AE9077-A813-4992-B5C9-B6B9EA4CFA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="195" windowWidth="28470" windowHeight="15240" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="1830" yWindow="1320" windowWidth="24660" windowHeight="12855" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1420,9 +1420,6 @@
   </si>
   <si>
     <t>d</t>
-  </si>
-  <si>
-    <t>Partially complete, some submeshes aren't drawing, it seems</t>
   </si>
 </sst>
 </file>
@@ -2039,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2231,7 +2228,7 @@
       <c r="C14" s="3">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2417,6 +2414,9 @@
       <c r="C30" s="3">
         <v>0</v>
       </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -2440,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>35</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>16</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>17</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>38</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>18</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>19</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>31</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>33</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>39</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>15</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2594,8 +2594,11 @@
       <c r="C46" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
@@ -2605,8 +2608,11 @@
       <c r="C47" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Added a point light to the second scene
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AE9077-A813-4992-B5C9-B6B9EA4CFA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF05F0A8-B62A-4831-94DB-4ECEB60499FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1320" windowWidth="24660" windowHeight="12855" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="300" yWindow="1440" windowWidth="24660" windowHeight="12855" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1419,7 +1419,7 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>d</t>
+    <t>Note: Level 2 has a yellow light in the center</t>
   </si>
 </sst>
 </file>
@@ -2036,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,6 +2242,9 @@
       <c r="C15" s="3">
         <v>0</v>
       </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" t="s">
         <v>50</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>7</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -2311,11 +2314,8 @@
       <c r="C21" s="3">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>12</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>34</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>47</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>48</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>13</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>21</v>
       </c>
@@ -2414,11 +2414,8 @@
       <c r="C30" s="3">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
@@ -2429,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
ChangeLevel() no longer re-initializes pipeline and shader modules.
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF05F0A8-B62A-4831-94DB-4ECEB60499FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD45D11-C16A-4910-9A07-C2532FC8D177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="1440" windowWidth="24660" windowHeight="12855" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1419,7 +1419,7 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>Note: Level 2 has a yellow light in the center</t>
+    <t>Note: Level 2 has a yellow point light in the center</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated rubric, added screen shot of scene 1
</commit_message>
<xml_diff>
--- a/NegronSierra_ProjectRubric.xlsx
+++ b/NegronSierra_ProjectRubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\attri\OneDrive\Desktop\GDBS\Mo. 14 DEV4\Week3\Level Renderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD45D11-C16A-4910-9A07-C2532FC8D177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B5E60A-5CA4-4162-8C81-CD58E041D609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="1440" windowWidth="24660" windowHeight="12855" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1417,9 +1417,6 @@
   </si>
   <si>
     <t>Complete</t>
-  </si>
-  <si>
-    <t>Note: Level 2 has a yellow point light in the center</t>
   </si>
 </sst>
 </file>
@@ -2034,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2043,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2057,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2068,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2085,7 +2082,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -2099,7 +2096,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -2113,7 +2110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2127,7 +2124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2141,7 +2138,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2155,7 +2152,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -2169,7 +2166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -2179,8 +2176,11 @@
       <c r="C10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>41</v>
       </c>
@@ -2245,11 +2245,8 @@
       <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>40</v>
       </c>

</xml_diff>